<commit_message>
Finish subsection on Good-Thomas
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HE YIMENG\Documents\Git Projects\PrimePower-NTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95FDDBF-1638-4DAD-A58B-C93E318DB6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A55B29-9A11-4694-9E64-A5AA10CB82EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
   </bookViews>
@@ -464,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F69820-EAB8-483A-9C1A-3660639291FD}">
   <dimension ref="A5:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +506,9 @@
       <c r="D6" s="1">
         <v>22247</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>239498</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -521,7 +523,9 @@
       <c r="D7" s="1">
         <v>22402</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>230037</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -534,7 +538,9 @@
       <c r="D8" s="1">
         <v>908</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>4193</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -549,7 +555,9 @@
       <c r="D9" s="1">
         <v>77</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>420</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -583,7 +591,9 @@
       <c r="D14" s="2">
         <v>30000</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2">
+        <v>100000</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
@@ -658,7 +668,9 @@
       <c r="D23" s="2">
         <v>30000</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2">
+        <v>100000</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">

</xml_diff>

<commit_message>
Complete experiment for p=2
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HE YIMENG\Documents\Git Projects\PrimePower-NTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A2FAA9-75F7-4850-AAE7-E4A7C136DEEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E71FCA7-F452-4B1A-BB2B-FA1B613D00B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
+    <workbookView xWindow="5295" yWindow="2550" windowWidth="19305" windowHeight="13050" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
   </bookViews>
   <sheets>
     <sheet name="prime 2" sheetId="1" r:id="rId1"/>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F69820-EAB8-483A-9C1A-3660639291FD}">
   <dimension ref="A5:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +711,9 @@
       <c r="D24" s="1">
         <v>133040</v>
       </c>
+      <c r="E24" s="1">
+        <v>2633100</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
@@ -722,6 +725,9 @@
       <c r="D25" s="1">
         <v>64871</v>
       </c>
+      <c r="E25" s="1">
+        <v>598649</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
@@ -733,6 +739,9 @@
       <c r="D26" s="1">
         <v>2249</v>
       </c>
+      <c r="E26" s="1">
+        <v>8314</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
@@ -743,6 +752,9 @@
       </c>
       <c r="D27" s="1">
         <v>139</v>
+      </c>
+      <c r="E27" s="1">
+        <v>666</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finish related work section
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HE YIMENG\Documents\Git Projects\PrimePower-NTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E71FCA7-F452-4B1A-BB2B-FA1B613D00B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E70A67-BB31-46D4-9C9D-549B871F4C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5295" yWindow="2550" windowWidth="19305" windowHeight="13050" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
   </bookViews>
   <sheets>
     <sheet name="prime 2" sheetId="1" r:id="rId1"/>
+    <sheet name="prime 31" sheetId="2" r:id="rId2"/>
+    <sheet name="prime 17" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="27">
   <si>
     <t>2^8</t>
   </si>
@@ -78,6 +80,45 @@
   </si>
   <si>
     <t>3^3 * 5 * 7 * 13 * 19</t>
+  </si>
+  <si>
+    <t>31^2</t>
+  </si>
+  <si>
+    <t>2^7 * 3 * 5</t>
+  </si>
+  <si>
+    <t>31^4</t>
+  </si>
+  <si>
+    <t>2^7 * 3 * 5 * 13</t>
+  </si>
+  <si>
+    <t>31^4 - 1</t>
+  </si>
+  <si>
+    <t>31^8</t>
+  </si>
+  <si>
+    <t>17^2</t>
+  </si>
+  <si>
+    <t>17^4 - 1</t>
+  </si>
+  <si>
+    <t>2^6 * 3^2 * 5</t>
+  </si>
+  <si>
+    <t>17^4</t>
+  </si>
+  <si>
+    <t>17^8</t>
+  </si>
+  <si>
+    <t>2^7 * 3^2 * 5 * 29</t>
+  </si>
+  <si>
+    <t>17^8 - 1</t>
   </si>
 </sst>
 </file>
@@ -470,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F69820-EAB8-483A-9C1A-3660639291FD}">
   <dimension ref="A5:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,4 +827,497 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F05C14-49A5-482B-97D9-9038F838E69A}">
+  <dimension ref="A5:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
+        <v>900</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>68.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7262</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>181</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3162</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1">
+        <v>662</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>41.6</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2">
+        <v>900</v>
+      </c>
+      <c r="D15" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>76.7</v>
+      </c>
+      <c r="D16" s="1">
+        <v>7206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>190</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="2">
+        <v>900</v>
+      </c>
+      <c r="D24" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>116</v>
+      </c>
+      <c r="D25" s="1">
+        <v>12588</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>244</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>66</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="D28" s="1">
+        <v>40.700000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1F0FC2-81EA-438B-9155-D97F9263E36C}">
+  <dimension ref="A5:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1">
+        <v>149945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>299</v>
+      </c>
+      <c r="D7" s="1">
+        <v>27015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>83</v>
+      </c>
+      <c r="D16" s="1">
+        <v>455928</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
+        <v>304</v>
+      </c>
+      <c r="D17" s="1">
+        <v>29573</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>43</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6527</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="D19" s="1">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D24" s="2">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>141</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1231909</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1">
+        <v>374</v>
+      </c>
+      <c r="D26" s="1">
+        <v>49495</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>66</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8520</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish Experiments and Conclusion section
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HE YIMENG\Documents\Git Projects\PrimePower-NTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E70A67-BB31-46D4-9C9D-549B871F4C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1260CAA-F662-43B8-BBE1-B5DC106D37F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{D1027F70-50BE-43E0-8DD8-0EB4F7074002}"/>
   </bookViews>
   <sheets>
     <sheet name="prime 2" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="31">
   <si>
     <t>2^8</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>17^8 - 1</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>37 * 73 * 109</t>
+  </si>
+  <si>
+    <t>13*37</t>
   </si>
 </sst>
 </file>
@@ -511,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F69820-EAB8-483A-9C1A-3660639291FD}">
   <dimension ref="A5:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D5" s="2">
         <v>30000</v>
@@ -547,7 +559,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>27</v>
+        <v>113</v>
       </c>
       <c r="D6" s="1">
         <v>22247</v>
@@ -564,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>490</v>
+        <v>509</v>
       </c>
       <c r="D7" s="1">
         <v>22402</v>
@@ -579,7 +591,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D8" s="1">
         <v>908</v>
@@ -596,7 +608,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1">
-        <v>1.4</v>
+        <v>2.9</v>
       </c>
       <c r="D9" s="1">
         <v>77</v>
@@ -623,6 +635,9 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
@@ -631,6 +646,20 @@
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>241</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -638,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D14" s="2">
         <v>30000</v>
@@ -652,7 +681,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>86</v>
+        <v>331</v>
       </c>
       <c r="D15" s="1">
         <v>64288</v>
@@ -666,7 +695,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="1">
-        <v>544</v>
+        <v>526</v>
       </c>
       <c r="D16" s="1">
         <v>28775</v>
@@ -680,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="1">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1">
         <v>1340</v>
@@ -694,7 +723,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="1">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1">
         <v>117</v>
@@ -733,7 +762,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="D23" s="2">
         <v>30000</v>
@@ -747,7 +776,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="1">
-        <v>144</v>
+        <v>608</v>
       </c>
       <c r="D24" s="1">
         <v>133040</v>
@@ -761,7 +790,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="1">
-        <v>990</v>
+        <v>972</v>
       </c>
       <c r="D25" s="1">
         <v>64871</v>
@@ -775,7 +804,7 @@
         <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="D26" s="1">
         <v>2249</v>
@@ -789,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="1">
-        <v>8.5</v>
+        <v>6.3</v>
       </c>
       <c r="D27" s="1">
         <v>139</v>
@@ -833,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3F05C14-49A5-482B-97D9-9038F838E69A}">
   <dimension ref="A5:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,6 +947,9 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
@@ -925,6 +957,14 @@
         <v>17</v>
       </c>
       <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1">
+        <v>37</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
@@ -1083,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1F0FC2-81EA-438B-9155-D97F9263E36C}">
   <dimension ref="A5:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,11 +1201,22 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="C12" s="1">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1">
+        <v>41761</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.35">

</xml_diff>